<commit_message>
updated code till faculty creation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AllCredsLogins_TestData.xlsx
+++ b/src/test/resources/testData/AllCredsLogins_TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t xml:space="preserve">TC No</t>
   </si>
@@ -96,6 +96,51 @@
   </si>
   <si>
     <t xml:space="preserve">onBoardUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChooseSubject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Occupation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConfirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faculty123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testFaculty@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupation</t>
   </si>
 </sst>
 </file>
@@ -199,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,6 +258,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,58 +444,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>8956895689</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
+      <c r="M2" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="sampleTestInstitute@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="sampleTestInstitute@gmail.com"/>
+    <hyperlink ref="G2" r:id="rId2" display="testFaculty@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
updated with 1 flow completely
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AllCredsLogins_TestData.xlsx
+++ b/src/test/resources/testData/AllCredsLogins_TestData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AllRoleLogins" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="OnboardingRegisteredInstitute" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="InstituteOnboardFacultyDetails" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t xml:space="preserve">TC No</t>
   </si>
@@ -147,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -185,6 +186,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -241,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,7 +265,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -266,12 +277,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -294,7 +309,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,8 +424,8 @@
   </sheetPr>
   <dimension ref="A1:XFC2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,7 +434,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.96"/>
@@ -430,108 +445,106 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="24.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16382" min="16382" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="XFB1" s="5"/>
-      <c r="XFC1" s="0"/>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="XFB1" s="6"/>
+      <c r="XFC1" s="1"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="8" t="n">
         <v>8956895689</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="K2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="XFB2" s="1"/>
-      <c r="XFC2" s="0"/>
+      <c r="XFC2" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -547,4 +560,136 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>8956895689</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="sampleTestInstitute@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId2" display="testFaculty@gmail.com"/>
+    <hyperlink ref="N2" r:id="rId3" display="testFaculty@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>